<commit_message>
Moved m1 out to remove an extra line and added norm. error graph
</commit_message>
<xml_diff>
--- a/graph_results.xlsx
+++ b/graph_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Documents\00-GMU\Spring 21\583\QuickSort-Bits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E944E6C7-967B-445F-959F-EE106B42194A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FDA9A-A81D-4CF9-AF5D-D55D56DD4487}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="469" xr2:uid="{BDDAB071-FA3D-4F20-B04F-C9EA0EA173A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
   <si>
     <t>Bits</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Average Bit Comparisons</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Normalized Difference</t>
   </si>
 </sst>
 </file>
@@ -1748,6 +1754,475 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Normalized Expectation Error</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.12320916905444126</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10473961380924517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11098198721673445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-BC51-40D0-9FB9-685F87ABC03F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.9312154610848687E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11562527801666617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0617812991337051E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-BC51-40D0-9FB9-685F87ABC03F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$9:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.18408992729712589</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1610034289430009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16314844772258486</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-BC51-40D0-9FB9-685F87ABC03F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$12:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.29769952487135382</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15560753448196757</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1731674609350497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-BC51-40D0-9FB9-685F87ABC03F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="593234608"/>
+        <c:axId val="593232312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="593234608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number of Bits</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593232312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="593232312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.30000000000000004"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Normalized Expectation Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593234608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3924,16 +4399,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>507205</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>30966</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>78582</xdr:rowOff>
+      <xdr:rowOff>35720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>250030</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>421491</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>107157</xdr:rowOff>
+      <xdr:rowOff>64295</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3960,16 +4435,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>578642</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>102403</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>88107</xdr:rowOff>
+      <xdr:rowOff>45245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>623887</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>147648</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>116682</xdr:rowOff>
+      <xdr:rowOff>73820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3996,16 +4471,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>511968</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>35720</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>35729</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>173833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>254793</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>426254</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>64295</xdr:rowOff>
+      <xdr:rowOff>21433</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4032,16 +4507,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>578643</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>102404</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>73820</xdr:rowOff>
+      <xdr:rowOff>30958</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142886</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>102395</xdr:rowOff>
+      <xdr:rowOff>59533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4061,6 +4536,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>338138</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B02B0A-5351-4A3B-8E63-CB7DB11789EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4366,10 +4877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2076243-A44D-49A7-ABB0-67CC26F14B6E}">
-  <dimension ref="B2:E35"/>
+  <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4377,9 +4888,11 @@
     <col min="3" max="3" width="19.73046875" customWidth="1"/>
     <col min="4" max="4" width="20.3984375" customWidth="1"/>
     <col min="5" max="5" width="22.265625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -4392,8 +4905,14 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>100</v>
       </c>
@@ -4406,8 +4925,16 @@
       <c r="E3">
         <v>1745</v>
       </c>
+      <c r="F3">
+        <f>E3-D3</f>
+        <v>215</v>
+      </c>
+      <c r="G3">
+        <f>F3/E3</f>
+        <v>0.12320916905444126</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>100</v>
       </c>
@@ -4420,8 +4947,16 @@
       <c r="E4">
         <v>1709</v>
       </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F14" si="0">E4-D4</f>
+        <v>179</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G14" si="1">F4/E4</f>
+        <v>0.10473961380924517</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>100</v>
       </c>
@@ -4434,8 +4969,16 @@
       <c r="E5">
         <v>1721</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.11098198721673445</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1000</v>
       </c>
@@ -4448,8 +4991,16 @@
       <c r="E6">
         <v>32391</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>2569</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>7.9312154610848687E-2</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1000</v>
       </c>
@@ -4462,8 +5013,16 @@
       <c r="E7">
         <v>33721</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3899</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.11562527801666617</v>
+      </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>1000</v>
       </c>
@@ -4476,8 +5035,16 @@
       <c r="E8">
         <v>32437</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2615</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>8.0617812991337051E-2</v>
+      </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>10000</v>
       </c>
@@ -4490,8 +5057,16 @@
       <c r="E9">
         <v>543995</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>100144</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.18408992729712589</v>
+      </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>10000</v>
       </c>
@@ -4504,8 +5079,16 @@
       <c r="E10">
         <v>529026</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>85175</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.1610034289430009</v>
+      </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>10000</v>
       </c>
@@ -4518,8 +5101,16 @@
       <c r="E11">
         <v>530382</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>86531</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.16314844772258486</v>
+      </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>20000</v>
       </c>
@@ -4532,8 +5123,16 @@
       <c r="E12">
         <v>1388887</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>413471</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.29769952487135382</v>
+      </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>20000</v>
       </c>
@@ -4546,8 +5145,16 @@
       <c r="E13">
         <v>1155169</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>179753</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.15560753448196757</v>
+      </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>20000</v>
       </c>
@@ -4560,16 +5167,33 @@
       <c r="E14">
         <v>1179702</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>204286</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.1731674609350497</v>
+      </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
       </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>100</v>
+      </c>
       <c r="C18">
         <v>10</v>
       </c>
@@ -4579,8 +5203,19 @@
       <c r="E18">
         <v>1745</v>
       </c>
+      <c r="F18">
+        <f>E18-D18</f>
+        <v>215</v>
+      </c>
+      <c r="G18">
+        <f>F18/E18</f>
+        <v>0.12320916905444126</v>
+      </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>100</v>
+      </c>
       <c r="C19">
         <v>15</v>
       </c>
@@ -4590,8 +5225,19 @@
       <c r="E19">
         <v>1709</v>
       </c>
+      <c r="F19">
+        <f t="shared" ref="F19:F20" si="2">E19-D19</f>
+        <v>179</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19:G20" si="3">F19/E19</f>
+        <v>0.10473961380924517</v>
+      </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>100</v>
+      </c>
       <c r="C20">
         <v>20</v>
       </c>
@@ -4601,16 +5247,30 @@
       <c r="E20">
         <v>1721</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.11098198721673445</v>
+      </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
         <v>2</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
       </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C23">
         <v>10</v>
       </c>
@@ -4620,8 +5280,16 @@
       <c r="E23">
         <v>32391</v>
       </c>
+      <c r="F23">
+        <f t="shared" ref="F23:F25" si="4">E23-D23</f>
+        <v>2569</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">F23/E23</f>
+        <v>7.9312154610848687E-2</v>
+      </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C24">
         <v>15</v>
       </c>
@@ -4631,8 +5299,16 @@
       <c r="E24">
         <v>33721</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>3899</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>0.11562527801666617</v>
+      </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C25">
         <v>20</v>
       </c>
@@ -4642,16 +5318,30 @@
       <c r="E25">
         <v>32437</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>2615</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>8.0617812991337051E-2</v>
+      </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D27" t="s">
         <v>2</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C28">
         <v>10</v>
       </c>
@@ -4661,8 +5351,16 @@
       <c r="E28">
         <v>543995</v>
       </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F30" si="6">E28-D28</f>
+        <v>100144</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="7">F28/E28</f>
+        <v>0.18408992729712589</v>
+      </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C29">
         <v>15</v>
       </c>
@@ -4672,8 +5370,16 @@
       <c r="E29">
         <v>529026</v>
       </c>
+      <c r="F29">
+        <f t="shared" si="6"/>
+        <v>85175</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="7"/>
+        <v>0.1610034289430009</v>
+      </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C30">
         <v>20</v>
       </c>
@@ -4683,16 +5389,30 @@
       <c r="E30">
         <v>530382</v>
       </c>
+      <c r="F30">
+        <f t="shared" si="6"/>
+        <v>86531</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="7"/>
+        <v>0.16314844772258486</v>
+      </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D32" t="s">
         <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
       </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C33">
         <v>10</v>
       </c>
@@ -4702,8 +5422,16 @@
       <c r="E33">
         <v>1388887</v>
       </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F35" si="8">E33-D33</f>
+        <v>413471</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G35" si="9">F33/E33</f>
+        <v>0.29769952487135382</v>
+      </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C34">
         <v>15</v>
       </c>
@@ -4713,8 +5441,16 @@
       <c r="E34">
         <v>1155169</v>
       </c>
+      <c r="F34">
+        <f t="shared" si="8"/>
+        <v>179753</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>0.15560753448196757</v>
+      </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C35">
         <v>20</v>
       </c>
@@ -4723,6 +5459,14 @@
       </c>
       <c r="E35">
         <v>1179702</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>204286</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>0.1731674609350497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel Graph Axis
</commit_message>
<xml_diff>
--- a/graph_results.xlsx
+++ b/graph_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Documents\00-GMU\Spring 21\583\QuickSort-Bits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FDA9A-A81D-4CF9-AF5D-D55D56DD4487}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE1BA1C-D0B6-4E3C-9804-D3F024BBA5D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="469" xr2:uid="{BDDAB071-FA3D-4F20-B04F-C9EA0EA173A7}"/>
   </bookViews>
@@ -382,6 +382,7 @@
         <c:axId val="653631592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -797,6 +798,7 @@
         <c:axId val="653564672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4880,7 +4882,7 @@
   <dimension ref="B2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>